<commit_message>
Added extra chartsheet testcases.
</commit_message>
<xml_diff>
--- a/xlsxwriter/test/comparison/xlsx_files/chartsheet08.xlsx
+++ b/xlsxwriter/test/comparison/xlsx_files/chartsheet08.xlsx
@@ -149,24 +149,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="46320256"/>
-        <c:axId val="46335872"/>
+        <c:axId val="61297792"/>
+        <c:axId val="61299328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="46320256"/>
+        <c:axId val="61297792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46335872"/>
+        <c:crossAx val="61299328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46335872"/>
+        <c:axId val="61299328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -174,7 +174,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46320256"/>
+        <c:crossAx val="61297792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -194,21 +194,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.55118110236220474" bottom="0.94488188976377963" header="0.11811023622047245" footer="0.11811023622047245"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
   <headerFooter>
-    <oddHeader>Page &amp;P</oddHeader>
-    <oddFooter>&amp;A</oddFooter>
+    <oddHeader>&amp;CPage &amp;P</oddHeader>
+    <oddFooter>&amp;C&amp;A</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9308969" cy="6078325"/>
+    <xdr:pos x="0" y="-47625"/>
+    <xdr:ext cx="6524625" cy="6124575"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>

</xml_diff>